<commit_message>
Updated Testsheet with ms
</commit_message>
<xml_diff>
--- a/p1/docs/al024-testsheet.xlsx
+++ b/p1/docs/al024-testsheet.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guga/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guga/ASA2021/p1/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{387D273F-C46D-9541-88ED-CBE954824896}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6355AD1B-4BF6-3443-B145-B70058254EF5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16020" xr2:uid="{93A3567E-400A-994D-8CA7-9B3B660EFBED}"/>
+    <workbookView xWindow="2220" yWindow="2860" windowWidth="28040" windowHeight="16020" xr2:uid="{93A3567E-400A-994D-8CA7-9B3B660EFBED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -410,64 +410,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0.01</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.01</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.7999999999999999E-2</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.5999999999999999E-2</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.9000000000000001E-2</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0999999999999997E-2</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.4999999999999998E-2</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.3999999999999999E-2</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.2E-2</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.9000000000000005E-2</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.09</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.109</c:v>
+                  <c:v>109</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.128</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.17499999999999999</c:v>
+                  <c:v>175</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.17899999999999999</c:v>
+                  <c:v>179</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.192</c:v>
+                  <c:v>192</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.20899999999999999</c:v>
+                  <c:v>209</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.23100000000000001</c:v>
+                  <c:v>231</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.28899999999999998</c:v>
+                  <c:v>289</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.3</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -532,8 +532,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Tamanho do Grafo</a:t>
+                  <a:t>Tamanho do Grafo (|V| +</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> |E|)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -649,7 +654,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Tempo de execução (seg)</a:t>
+                  <a:t>Tempo de execução (ms)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1673,7 +1678,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1713,7 +1718,8 @@
         <v>2054</v>
       </c>
       <c r="E2">
-        <v>0.01</v>
+        <f>1000*0.01</f>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1731,7 +1737,8 @@
         <v>8123</v>
       </c>
       <c r="E3">
-        <v>0.01</v>
+        <f>1000*0.01</f>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1749,7 +1756,8 @@
         <v>18212</v>
       </c>
       <c r="E4">
-        <v>1.7999999999999999E-2</v>
+        <f>1000*0.018</f>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1767,7 +1775,9 @@
         <v>32241</v>
       </c>
       <c r="E5">
-        <v>2.5999999999999999E-2</v>
+        <f>1000*
+0.026</f>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1785,7 +1795,8 @@
         <v>50583</v>
       </c>
       <c r="E6">
-        <v>2.9000000000000001E-2</v>
+        <f>1000*0.029</f>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1803,7 +1814,8 @@
         <v>72512</v>
       </c>
       <c r="E7">
-        <v>5.0999999999999997E-2</v>
+        <f>1000*0.051</f>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1821,7 +1833,8 @@
         <v>98449</v>
       </c>
       <c r="E8">
-        <v>4.4999999999999998E-2</v>
+        <f>1000*0.045</f>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1839,7 +1852,8 @@
         <v>128477</v>
       </c>
       <c r="E9">
-        <v>5.3999999999999999E-2</v>
+        <f>1000*0.054</f>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1857,7 +1871,8 @@
         <v>162829</v>
       </c>
       <c r="E10">
-        <v>6.2E-2</v>
+        <f>1000*0.062</f>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1875,7 +1890,8 @@
         <v>200819</v>
       </c>
       <c r="E11">
-        <v>9.9000000000000005E-2</v>
+        <f>1000*0.099</f>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1893,7 +1909,8 @@
         <v>242341</v>
       </c>
       <c r="E12">
-        <v>0.09</v>
+        <f>1000*0.09</f>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1911,7 +1928,8 @@
         <v>289329</v>
       </c>
       <c r="E13">
-        <v>0.109</v>
+        <f>1000*0.109</f>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1929,7 +1947,8 @@
         <v>338827</v>
       </c>
       <c r="E14">
-        <v>0.128</v>
+        <f>1000*0.128</f>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1947,7 +1966,8 @@
         <v>393074</v>
       </c>
       <c r="E15">
-        <v>0.17499999999999999</v>
+        <f>1000*0.175</f>
+        <v>175</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1965,7 +1985,8 @@
         <v>451231</v>
       </c>
       <c r="E16">
-        <v>0.17899999999999999</v>
+        <f>1000*0.179</f>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1983,7 +2004,8 @@
         <v>513626</v>
       </c>
       <c r="E17">
-        <v>0.192</v>
+        <f>1000*0.192</f>
+        <v>192</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -2001,7 +2023,8 @@
         <v>579565</v>
       </c>
       <c r="E18">
-        <v>0.20899999999999999</v>
+        <f>1000*0.209</f>
+        <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -2019,7 +2042,8 @@
         <v>649761</v>
       </c>
       <c r="E19">
-        <v>0.23100000000000001</v>
+        <f>1000*0.231</f>
+        <v>231</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -2037,7 +2061,8 @@
         <v>723921</v>
       </c>
       <c r="E20">
-        <v>0.28899999999999998</v>
+        <f>1000*0.289</f>
+        <v>289</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -2055,7 +2080,8 @@
         <v>802742</v>
       </c>
       <c r="E21">
-        <v>0.3</v>
+        <f>1000*0.3</f>
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added updated version of p2 report
</commit_message>
<xml_diff>
--- a/p1/docs/al024-testsheet.xlsx
+++ b/p1/docs/al024-testsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guga/ASA2021/p1/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6355AD1B-4BF6-3443-B145-B70058254EF5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1753F7DE-D34C-1F48-BE0C-A1C6CC46BCFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="2860" windowWidth="28040" windowHeight="16020" xr2:uid="{93A3567E-400A-994D-8CA7-9B3B660EFBED}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="15980" xr2:uid="{93A3567E-400A-994D-8CA7-9B3B660EFBED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1678,12 +1678,13 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="D1" sqref="D1:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="17.83203125" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -1733,7 +1734,7 @@
         <v>7923</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D21" si="0">B3+C3</f>
+        <f>B3+C3</f>
         <v>8123</v>
       </c>
       <c r="E3">
@@ -1752,7 +1753,7 @@
         <v>17912</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" si="0"/>
+        <f>B4+C4</f>
         <v>18212</v>
       </c>
       <c r="E4">
@@ -1771,7 +1772,7 @@
         <v>31841</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" si="0"/>
+        <f>B5+C5</f>
         <v>32241</v>
       </c>
       <c r="E5">
@@ -1791,7 +1792,7 @@
         <v>50083</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" si="0"/>
+        <f>B6+C6</f>
         <v>50583</v>
       </c>
       <c r="E6">
@@ -1810,7 +1811,7 @@
         <v>71912</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" si="0"/>
+        <f>B7+C7</f>
         <v>72512</v>
       </c>
       <c r="E7">
@@ -1829,7 +1830,7 @@
         <v>97749</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" si="0"/>
+        <f>B8+C8</f>
         <v>98449</v>
       </c>
       <c r="E8">
@@ -1848,7 +1849,7 @@
         <v>127677</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" si="0"/>
+        <f>B9+C9</f>
         <v>128477</v>
       </c>
       <c r="E9">
@@ -1867,7 +1868,7 @@
         <v>161929</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" si="0"/>
+        <f>B10+C10</f>
         <v>162829</v>
       </c>
       <c r="E10">
@@ -1886,7 +1887,7 @@
         <v>199819</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="0"/>
+        <f>B11+C11</f>
         <v>200819</v>
       </c>
       <c r="E11">
@@ -1905,7 +1906,7 @@
         <v>241241</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" si="0"/>
+        <f>B12+C12</f>
         <v>242341</v>
       </c>
       <c r="E12">
@@ -1924,7 +1925,7 @@
         <v>288129</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" si="0"/>
+        <f>B13+C13</f>
         <v>289329</v>
       </c>
       <c r="E13">
@@ -1943,7 +1944,7 @@
         <v>337527</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" si="0"/>
+        <f>B14+C14</f>
         <v>338827</v>
       </c>
       <c r="E14">
@@ -1962,7 +1963,7 @@
         <v>391674</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="0"/>
+        <f>B15+C15</f>
         <v>393074</v>
       </c>
       <c r="E15">
@@ -1981,7 +1982,7 @@
         <v>449731</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" si="0"/>
+        <f>B16+C16</f>
         <v>451231</v>
       </c>
       <c r="E16">
@@ -2000,7 +2001,7 @@
         <v>512026</v>
       </c>
       <c r="D17" s="1">
-        <f t="shared" si="0"/>
+        <f>B17+C17</f>
         <v>513626</v>
       </c>
       <c r="E17">
@@ -2019,7 +2020,7 @@
         <v>577865</v>
       </c>
       <c r="D18" s="1">
-        <f t="shared" si="0"/>
+        <f>B18+C18</f>
         <v>579565</v>
       </c>
       <c r="E18">
@@ -2038,7 +2039,7 @@
         <v>647961</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" si="0"/>
+        <f>B19+C19</f>
         <v>649761</v>
       </c>
       <c r="E19">
@@ -2057,7 +2058,7 @@
         <v>722021</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" si="0"/>
+        <f>B20+C20</f>
         <v>723921</v>
       </c>
       <c r="E20">
@@ -2076,7 +2077,7 @@
         <v>800742</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="0"/>
+        <f>B21+C21</f>
         <v>802742</v>
       </c>
       <c r="E21">

</xml_diff>